<commit_message>
1. 加入MyUser Model 2. 修改一下base.html假装不是剽窃
</commit_message>
<xml_diff>
--- a/数据库架构说明.xlsx
+++ b/数据库架构说明.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8940" windowHeight="6720" tabRatio="629" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8940" windowHeight="6720" tabRatio="629" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Answer" sheetId="7" r:id="rId6"/>
     <sheet name="Grade" sheetId="10" r:id="rId7"/>
     <sheet name="User" sheetId="6" r:id="rId8"/>
+    <sheet name="MyUser" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="147">
   <si>
     <t>学生表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -548,6 +549,50 @@
   </si>
   <si>
     <t>正确次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MyUser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自加字段 OneToOne - User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nickname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>authority</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限 0学生1教师2管理员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1041,7 +1086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1849,4 +1894,70 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>